<commit_message>
Added a way to insert arbitrary data about the root instance in the ExcelTableFile_FromTemplate.cs. Changed Table<T> to be a record because i want to use the 'with' syntax
</commit_message>
<xml_diff>
--- a/src/rambap.cplx.UnitTests/ExcelTemplates/CplxCostingTemplate.xlsx
+++ b/src/rambap.cplx.UnitTests/ExcelTemplates/CplxCostingTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baram\Desktop\Repo\rambap.cplx\src\rambap.cplx.UnitTests\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A1A66D-D18E-4790-8BEE-EBF486751E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89E0E3-33C7-4AA3-94E3-27D8FCC38BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="1110" windowWidth="16410" windowHeight="14520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6315" yWindow="1815" windowWidth="16410" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>#</t>
   </si>
@@ -63,14 +63,34 @@
   </si>
   <si>
     <t>Task Total Duration</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>GenDate</t>
+  </si>
+  <si>
+    <t>Info :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -150,12 +170,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,12 +457,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -507,7 +557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2419FDE-2CFE-43BC-8A92-3829A6897956}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>

</xml_diff>